<commit_message>
Adding changes corresponding to - Listeners, Annotation, Data Provider and Test Data Supplier
</commit_message>
<xml_diff>
--- a/src/test/resources/data/user-login.xlsx
+++ b/src/test/resources/data/user-login.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="login-credentials" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -59,7 +58,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -67,28 +66,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,12 +376,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I5"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -444,86 +428,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:C18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>